<commit_message>
excluded scene bug fix
</commit_message>
<xml_diff>
--- a/Projects/PNGAMERICA/Data/Template_v4.4.xlsx
+++ b/Projects/PNGAMERICA/Data/Template_v4.4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="block and availability" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,6 +44,9 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
@@ -56,6 +59,9 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="dfg" vbProcedure="false">main!$A$1:$F$194</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="qwe" vbProcedure="false">main!$A$1:$F$194</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="sdf" vbProcedure="false">main!$A$1:$F$211</definedName>
@@ -85,17 +91,20 @@
     <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$440</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">main!$A$1:$F$434</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">main!$A$1:$F$440</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">main!$A$1:$F$434</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$368</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$368</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -107,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4198" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4220" uniqueCount="224">
   <si>
     <t>kpi Name</t>
   </si>
@@ -604,7 +613,7 @@
     <t>Adjacency:Naturals Adjacency:FABRICARE:NATURALS=GREEN:BENEFIT=FREE/SENSITIVE</t>
   </si>
   <si>
-    <t>Orchestration:SUD_Horiz_Orches:FABRIC_CARE:SEG=LAUNDRY CARE:FORM=LAUNDRY UNIT DOSE</t>
+    <t>Orchestration:SUD_Horiz_Orches:FABRICARE:SEG=LAUNDRY CARE:FORM=LAUNDRY UNIT DOSE</t>
   </si>
   <si>
     <t>sud_orchestration</t>
@@ -649,15 +658,39 @@
     <t>custom orchestration</t>
   </si>
   <si>
+    <t>attribute_1</t>
+  </si>
+  <si>
+    <t>filter attribute 1</t>
+  </si>
+  <si>
+    <t>attribute_2</t>
+  </si>
+  <si>
+    <t>filter attribute 2</t>
+  </si>
+  <si>
     <t>ECONOMY, PREMIUM, SUPER PREMIUM</t>
   </si>
   <si>
     <t>top, bottom</t>
   </si>
   <si>
+    <t>ALWAYS</t>
+  </si>
+  <si>
+    <t>PADS</t>
+  </si>
+  <si>
     <t>y</t>
   </si>
   <si>
+    <t>TAMPAX</t>
+  </si>
+  <si>
+    <t>TAMPONS</t>
+  </si>
+  <si>
     <t>1 - REGULAR, 2 - LONG SUPER, 3 - EXTRA LONG SUPER, 4 - OVERNIGHT, 5 - EXTRA HEAVY OVERNIGHT</t>
   </si>
   <si>
@@ -673,12 +706,6 @@
     <t>ABSORBENCY</t>
   </si>
   <si>
-    <t>ALWAYS</t>
-  </si>
-  <si>
-    <t>TAMPAX</t>
-  </si>
-  <si>
     <t>Group 1 param</t>
   </si>
   <si>
@@ -725,6 +752,9 @@
   </si>
   <si>
     <t>bottom</t>
+  </si>
+  <si>
+    <t>custom</t>
   </si>
   <si>
     <t>LAUNDRY UNIT DOSE</t>
@@ -1549,19 +1579,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O11" activeCellId="0" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="99.2995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="101.975708502024"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
         <v>16</v>
       </c>
@@ -1583,8 +1613,20 @@
       <c r="G1" s="0" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H1" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
         <v>152</v>
       </c>
@@ -1592,19 +1634,31 @@
         <v>21</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>52</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
         <v>154</v>
       </c>
@@ -1612,22 +1666,34 @@
         <v>21</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D3" s="24" t="s">
         <v>52</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>188</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
         <v>155</v>
       </c>
@@ -1635,19 +1701,31 @@
         <v>21</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>52</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
         <v>156</v>
       </c>
@@ -1655,19 +1733,31 @@
         <v>21</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>52</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>39</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,13 +1768,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1695,13 +1785,13 @@
         <v>29</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1762,7 +1852,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>22</v>
@@ -1787,15 +1877,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J37" activeCellId="0" sqref="J37"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.0890688259109"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="74.0202429149798"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1804,52 +1894,55 @@
         <v>16</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="M1" s="26" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="N1" s="27" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="O1" s="27" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="P1" s="27" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="Q1" s="27" t="s">
-        <v>205</v>
+        <v>211</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,37 +1953,37 @@
         <v>26</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>26</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>22</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="P2" s="0" t="n">
         <v>1</v>
@@ -1907,20 +2000,23 @@
         <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D3" s="28"/>
       <c r="H3" s="28" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="N3" s="28" t="n">
         <v>1</v>
       </c>
       <c r="O3" s="28" t="n">
         <v>1</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1931,13 +2027,13 @@
         <v>26</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>26</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>1</v>
@@ -1963,10 +2059,10 @@
         <v>7</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>1</v>
@@ -2064,8 +2160,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="88.6963562753036"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="91.0526315789474"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.914979757085"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -2539,8 +2635,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="82.4817813765182"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.4493927125506"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="84.6234817813765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.3765182186235"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -3720,7 +3816,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="99.5141700404858"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="102.19028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -5833,8 +5929,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3805668016194"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
@@ -7923,12 +8019,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.4493927125506"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.0566801619433"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -8484,23 +8580,23 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F441"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B70" activeCellId="0" sqref="B70"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A349" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B375" activeCellId="0" sqref="B375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="98.2267206477733"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.2712550607288"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="100.797570850202"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="68.8785425101215"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -8524,7 +8620,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>127</v>
       </c>
@@ -8541,7 +8637,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
         <v>127</v>
       </c>
@@ -8558,7 +8654,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>127</v>
       </c>
@@ -8575,7 +8671,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
         <v>127</v>
       </c>
@@ -8592,7 +8688,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
         <v>127</v>
       </c>
@@ -8609,7 +8705,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
         <v>127</v>
       </c>
@@ -8626,7 +8722,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
         <v>127</v>
       </c>
@@ -8643,7 +8739,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
         <v>127</v>
       </c>
@@ -8660,7 +8756,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
         <v>127</v>
       </c>
@@ -8677,7 +8773,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
         <v>127</v>
       </c>
@@ -8728,7 +8824,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
         <v>127</v>
       </c>
@@ -8745,7 +8841,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
         <v>127</v>
       </c>
@@ -8762,7 +8858,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
         <v>127</v>
       </c>
@@ -8779,7 +8875,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
         <v>127</v>
       </c>
@@ -8796,7 +8892,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -8813,7 +8909,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
         <v>127</v>
       </c>
@@ -8830,7 +8926,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
         <v>127</v>
       </c>
@@ -8847,7 +8943,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
         <v>127</v>
       </c>
@@ -8864,7 +8960,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
         <v>127</v>
       </c>
@@ -8881,7 +8977,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
         <v>127</v>
       </c>
@@ -8898,7 +8994,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
         <v>127</v>
       </c>
@@ -8915,7 +9011,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
         <v>127</v>
       </c>
@@ -8932,7 +9028,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
         <v>127</v>
       </c>
@@ -8949,7 +9045,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
         <v>127</v>
       </c>
@@ -8966,7 +9062,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
         <v>127</v>
       </c>
@@ -8983,7 +9079,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
         <v>127</v>
       </c>
@@ -9000,7 +9096,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
         <v>127</v>
       </c>
@@ -9017,7 +9113,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
         <v>127</v>
       </c>
@@ -9034,7 +9130,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
         <v>127</v>
       </c>
@@ -9051,7 +9147,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
         <v>127</v>
       </c>
@@ -9068,7 +9164,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
         <v>127</v>
       </c>
@@ -9085,7 +9181,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
         <v>127</v>
       </c>
@@ -9238,7 +9334,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="s">
         <v>127</v>
       </c>
@@ -9255,7 +9351,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="s">
         <v>127</v>
       </c>
@@ -9272,7 +9368,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="s">
         <v>127</v>
       </c>
@@ -9289,7 +9385,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>139</v>
       </c>
@@ -9306,7 +9402,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
         <v>127</v>
       </c>
@@ -9323,7 +9419,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
         <v>127</v>
       </c>
@@ -9340,7 +9436,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
         <v>127</v>
       </c>
@@ -9357,7 +9453,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="s">
         <v>127</v>
       </c>
@@ -9374,7 +9470,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="s">
         <v>127</v>
       </c>
@@ -9391,7 +9487,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="11" t="s">
         <v>127</v>
       </c>
@@ -9408,7 +9504,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>139</v>
       </c>
@@ -9425,7 +9521,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>139</v>
       </c>
@@ -9442,7 +9538,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>139</v>
       </c>
@@ -9459,7 +9555,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>139</v>
       </c>
@@ -9476,7 +9572,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>139</v>
       </c>
@@ -9493,7 +9589,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>144</v>
       </c>
@@ -9510,7 +9606,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>144</v>
       </c>
@@ -9527,7 +9623,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>144</v>
       </c>
@@ -9544,7 +9640,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>144</v>
       </c>
@@ -9561,7 +9657,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>144</v>
       </c>
@@ -9578,7 +9674,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="11" t="s">
         <v>146</v>
       </c>
@@ -9595,7 +9691,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="11" t="s">
         <v>146</v>
       </c>
@@ -9612,7 +9708,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="11" t="s">
         <v>146</v>
       </c>
@@ -9629,7 +9725,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="11" t="s">
         <v>146</v>
       </c>
@@ -9646,7 +9742,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="11" t="s">
         <v>146</v>
       </c>
@@ -9697,7 +9793,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="11" t="s">
         <v>146</v>
       </c>
@@ -9714,7 +9810,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="11" t="s">
         <v>146</v>
       </c>
@@ -9731,7 +9827,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="11" t="s">
         <v>146</v>
       </c>
@@ -9748,7 +9844,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="11" t="s">
         <v>146</v>
       </c>
@@ -9765,7 +9861,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="11" t="s">
         <v>146</v>
       </c>
@@ -9782,7 +9878,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="11" t="s">
         <v>146</v>
       </c>
@@ -9799,7 +9895,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="11" t="s">
         <v>146</v>
       </c>
@@ -9816,7 +9912,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="11" t="s">
         <v>146</v>
       </c>
@@ -9833,7 +9929,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="11" t="s">
         <v>146</v>
       </c>
@@ -9850,7 +9946,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="11" t="s">
         <v>146</v>
       </c>
@@ -9867,7 +9963,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="11" t="s">
         <v>146</v>
       </c>
@@ -9884,7 +9980,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="11" t="s">
         <v>146</v>
       </c>
@@ -9901,7 +9997,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="11" t="s">
         <v>146</v>
       </c>
@@ -9918,7 +10014,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="11" t="s">
         <v>146</v>
       </c>
@@ -9935,7 +10031,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="11" t="s">
         <v>146</v>
       </c>
@@ -9952,7 +10048,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="11" t="s">
         <v>146</v>
       </c>
@@ -9969,7 +10065,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="11" t="s">
         <v>146</v>
       </c>
@@ -9986,7 +10082,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="11" t="s">
         <v>146</v>
       </c>
@@ -10003,7 +10099,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="11" t="s">
         <v>146</v>
       </c>
@@ -10020,7 +10116,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="11" t="s">
         <v>146</v>
       </c>
@@ -10037,7 +10133,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="11" t="s">
         <v>146</v>
       </c>
@@ -10054,7 +10150,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="11" t="s">
         <v>146</v>
       </c>
@@ -10207,7 +10303,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="11" t="s">
         <v>146</v>
       </c>
@@ -10224,7 +10320,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="11" t="s">
         <v>146</v>
       </c>
@@ -10241,7 +10337,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="11" t="s">
         <v>146</v>
       </c>
@@ -10258,7 +10354,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>139</v>
       </c>
@@ -10275,7 +10371,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>139</v>
       </c>
@@ -10292,7 +10388,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>139</v>
       </c>
@@ -10309,7 +10405,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>139</v>
       </c>
@@ -10326,7 +10422,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>139</v>
       </c>
@@ -10343,7 +10439,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>139</v>
       </c>
@@ -10360,7 +10456,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>139</v>
       </c>
@@ -10377,7 +10473,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>139</v>
       </c>
@@ -10394,7 +10490,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>139</v>
       </c>
@@ -10411,7 +10507,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>139</v>
       </c>
@@ -10428,7 +10524,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>139</v>
       </c>
@@ -10445,7 +10541,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>139</v>
       </c>
@@ -10462,7 +10558,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>139</v>
       </c>
@@ -10479,7 +10575,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>139</v>
       </c>
@@ -10496,7 +10592,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>139</v>
       </c>
@@ -10513,7 +10609,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>139</v>
       </c>
@@ -10530,7 +10626,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>139</v>
       </c>
@@ -10547,7 +10643,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>139</v>
       </c>
@@ -10564,7 +10660,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>139</v>
       </c>
@@ -10581,7 +10677,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
         <v>139</v>
       </c>
@@ -10598,7 +10694,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>139</v>
       </c>
@@ -10615,7 +10711,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>139</v>
       </c>
@@ -10632,7 +10728,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>139</v>
       </c>
@@ -10649,7 +10745,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
         <v>139</v>
       </c>
@@ -10666,7 +10762,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>139</v>
       </c>
@@ -10683,7 +10779,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>139</v>
       </c>
@@ -10700,7 +10796,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>139</v>
       </c>
@@ -10717,7 +10813,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>139</v>
       </c>
@@ -10734,7 +10830,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>139</v>
       </c>
@@ -10751,7 +10847,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>139</v>
       </c>
@@ -10768,7 +10864,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>144</v>
       </c>
@@ -10785,7 +10881,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>144</v>
       </c>
@@ -10802,7 +10898,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>144</v>
       </c>
@@ -10819,7 +10915,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
         <v>144</v>
       </c>
@@ -10836,7 +10932,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
         <v>144</v>
       </c>
@@ -10853,7 +10949,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
         <v>144</v>
       </c>
@@ -10870,7 +10966,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
         <v>144</v>
       </c>
@@ -10887,7 +10983,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>144</v>
       </c>
@@ -10904,7 +11000,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
         <v>144</v>
       </c>
@@ -10921,7 +11017,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
         <v>144</v>
       </c>
@@ -10938,7 +11034,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
         <v>144</v>
       </c>
@@ -10955,7 +11051,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
         <v>144</v>
       </c>
@@ -10972,7 +11068,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
         <v>144</v>
       </c>
@@ -10989,7 +11085,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>144</v>
       </c>
@@ -11006,7 +11102,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="11" t="s">
         <v>127</v>
       </c>
@@ -11023,7 +11119,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
         <v>144</v>
       </c>
@@ -11040,7 +11136,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="11" t="s">
         <v>127</v>
       </c>
@@ -11057,7 +11153,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="11" t="s">
         <v>127</v>
       </c>
@@ -11074,7 +11170,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="11" t="s">
         <v>127</v>
       </c>
@@ -11091,7 +11187,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="11" t="s">
         <v>127</v>
       </c>
@@ -11108,7 +11204,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
         <v>144</v>
       </c>
@@ -11125,7 +11221,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="11" t="s">
         <v>127</v>
       </c>
@@ -11142,7 +11238,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="11" t="s">
         <v>127</v>
       </c>
@@ -11159,7 +11255,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="11" t="s">
         <v>127</v>
       </c>
@@ -11176,7 +11272,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="11" t="s">
         <v>127</v>
       </c>
@@ -11193,7 +11289,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="11" t="s">
         <v>127</v>
       </c>
@@ -11210,7 +11306,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="11" t="s">
         <v>127</v>
       </c>
@@ -11227,7 +11323,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="11" t="s">
         <v>127</v>
       </c>
@@ -11244,7 +11340,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="11" t="s">
         <v>127</v>
       </c>
@@ -11261,7 +11357,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="11" t="s">
         <v>127</v>
       </c>
@@ -11278,7 +11374,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="11" t="s">
         <v>127</v>
       </c>
@@ -11295,7 +11391,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="11" t="s">
         <v>127</v>
       </c>
@@ -11312,7 +11408,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="11" t="s">
         <v>146</v>
       </c>
@@ -11329,7 +11425,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="11" t="s">
         <v>146</v>
       </c>
@@ -11346,7 +11442,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="11" t="s">
         <v>146</v>
       </c>
@@ -11363,7 +11459,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="11" t="s">
         <v>146</v>
       </c>
@@ -11380,7 +11476,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="11" t="s">
         <v>146</v>
       </c>
@@ -11397,7 +11493,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
         <v>139</v>
       </c>
@@ -11414,7 +11510,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
         <v>139</v>
       </c>
@@ -11431,7 +11527,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
         <v>139</v>
       </c>
@@ -11448,7 +11544,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
         <v>139</v>
       </c>
@@ -11465,7 +11561,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
         <v>139</v>
       </c>
@@ -11482,7 +11578,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
         <v>144</v>
       </c>
@@ -11499,7 +11595,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
         <v>144</v>
       </c>
@@ -11516,7 +11612,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
         <v>144</v>
       </c>
@@ -11533,7 +11629,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
         <v>144</v>
       </c>
@@ -11550,7 +11646,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
         <v>144</v>
       </c>
@@ -11771,7 +11867,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
         <v>139</v>
       </c>
@@ -11788,7 +11884,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
         <v>139</v>
       </c>
@@ -11805,7 +11901,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
         <v>144</v>
       </c>
@@ -11822,7 +11918,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
         <v>144</v>
       </c>
@@ -11839,7 +11935,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
         <v>144</v>
       </c>
@@ -11856,7 +11952,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
         <v>144</v>
       </c>
@@ -11873,7 +11969,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
         <v>139</v>
       </c>
@@ -11890,7 +11986,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
         <v>139</v>
       </c>
@@ -11907,7 +12003,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
         <v>139</v>
       </c>
@@ -11924,7 +12020,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
         <v>139</v>
       </c>
@@ -11941,7 +12037,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
         <v>139</v>
       </c>
@@ -11958,7 +12054,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
         <v>139</v>
       </c>
@@ -11975,7 +12071,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="11" t="s">
         <v>146</v>
       </c>
@@ -11992,7 +12088,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="11" t="s">
         <v>146</v>
       </c>
@@ -12009,7 +12105,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="11" t="s">
         <v>146</v>
       </c>
@@ -12026,7 +12122,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="11" t="s">
         <v>146</v>
       </c>
@@ -12043,7 +12139,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="11" t="s">
         <v>146</v>
       </c>
@@ -12060,7 +12156,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="11" t="s">
         <v>146</v>
       </c>
@@ -12077,7 +12173,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
         <v>139</v>
       </c>
@@ -12094,7 +12190,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
         <v>139</v>
       </c>
@@ -12111,7 +12207,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
         <v>144</v>
       </c>
@@ -12128,7 +12224,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
         <v>144</v>
       </c>
@@ -12145,7 +12241,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
         <v>144</v>
       </c>
@@ -12162,7 +12258,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
         <v>144</v>
       </c>
@@ -12179,7 +12275,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
         <v>144</v>
       </c>
@@ -12196,7 +12292,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
         <v>144</v>
       </c>
@@ -12213,7 +12309,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
         <v>144</v>
       </c>
@@ -12230,7 +12326,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
         <v>144</v>
       </c>
@@ -12247,7 +12343,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
         <v>144</v>
       </c>
@@ -12264,7 +12360,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
         <v>144</v>
       </c>
@@ -12281,7 +12377,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
         <v>144</v>
       </c>
@@ -12298,7 +12394,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
         <v>144</v>
       </c>
@@ -12315,7 +12411,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="11" t="s">
         <v>127</v>
       </c>
@@ -12332,7 +12428,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="11" t="s">
         <v>146</v>
       </c>
@@ -12349,7 +12445,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
         <v>144</v>
       </c>
@@ -12366,7 +12462,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
         <v>144</v>
       </c>
@@ -12383,7 +12479,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
         <v>144</v>
       </c>
@@ -12400,7 +12496,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
         <v>144</v>
       </c>
@@ -12417,7 +12513,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
         <v>144</v>
       </c>
@@ -12434,7 +12530,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
         <v>144</v>
       </c>
@@ -12451,7 +12547,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
         <v>144</v>
       </c>
@@ -12468,7 +12564,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
         <v>144</v>
       </c>
@@ -12485,7 +12581,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
         <v>144</v>
       </c>
@@ -12502,7 +12598,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
         <v>144</v>
       </c>
@@ -12519,7 +12615,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
         <v>144</v>
       </c>
@@ -12536,7 +12632,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="238" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
         <v>144</v>
       </c>
@@ -12553,7 +12649,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="239" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
         <v>144</v>
       </c>
@@ -12570,7 +12666,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
         <v>144</v>
       </c>
@@ -12587,7 +12683,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
         <v>144</v>
       </c>
@@ -12604,7 +12700,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
         <v>144</v>
       </c>
@@ -12621,7 +12717,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
         <v>144</v>
       </c>
@@ -12638,7 +12734,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
         <v>144</v>
       </c>
@@ -12655,7 +12751,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
         <v>144</v>
       </c>
@@ -12672,7 +12768,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
         <v>144</v>
       </c>
@@ -12689,7 +12785,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
         <v>144</v>
       </c>
@@ -12706,7 +12802,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
         <v>144</v>
       </c>
@@ -12723,7 +12819,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="249" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
         <v>144</v>
       </c>
@@ -12740,7 +12836,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="250" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
         <v>144</v>
       </c>
@@ -12757,7 +12853,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
         <v>144</v>
       </c>
@@ -12774,7 +12870,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
         <v>144</v>
       </c>
@@ -12791,7 +12887,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
         <v>144</v>
       </c>
@@ -12808,7 +12904,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
         <v>144</v>
       </c>
@@ -12825,7 +12921,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
         <v>144</v>
       </c>
@@ -12842,7 +12938,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
         <v>144</v>
       </c>
@@ -12859,7 +12955,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
         <v>144</v>
       </c>
@@ -12876,7 +12972,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
         <v>144</v>
       </c>
@@ -12893,7 +12989,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
         <v>144</v>
       </c>
@@ -12910,7 +13006,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
         <v>144</v>
       </c>
@@ -12927,7 +13023,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
         <v>144</v>
       </c>
@@ -12944,7 +13040,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
         <v>144</v>
       </c>
@@ -12961,7 +13057,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
         <v>144</v>
       </c>
@@ -12978,7 +13074,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
         <v>144</v>
       </c>
@@ -12995,7 +13091,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
         <v>144</v>
       </c>
@@ -13012,7 +13108,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
         <v>144</v>
       </c>
@@ -13029,7 +13125,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
         <v>144</v>
       </c>
@@ -13046,7 +13142,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
         <v>144</v>
       </c>
@@ -13063,7 +13159,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="269" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
         <v>144</v>
       </c>
@@ -13080,7 +13176,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
         <v>144</v>
       </c>
@@ -13097,7 +13193,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
         <v>144</v>
       </c>
@@ -13114,7 +13210,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
         <v>144</v>
       </c>
@@ -13131,7 +13227,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
         <v>144</v>
       </c>
@@ -13148,7 +13244,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
         <v>144</v>
       </c>
@@ -13165,7 +13261,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="275" s="20" customFormat="true" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" s="20" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="20" t="s">
         <v>144</v>
       </c>
@@ -13182,7 +13278,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
         <v>144</v>
       </c>
@@ -13199,7 +13295,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="277" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
         <v>144</v>
       </c>
@@ -13216,7 +13312,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
         <v>144</v>
       </c>
@@ -13233,7 +13329,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="279" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="279" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
         <v>144</v>
       </c>
@@ -13250,7 +13346,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
         <v>144</v>
       </c>
@@ -13267,7 +13363,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="281" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="281" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
         <v>144</v>
       </c>
@@ -13284,7 +13380,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="282" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
         <v>144</v>
       </c>
@@ -13301,7 +13397,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="283" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
         <v>144</v>
       </c>
@@ -13318,7 +13414,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
         <v>144</v>
       </c>
@@ -13335,7 +13431,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="285" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
         <v>144</v>
       </c>
@@ -13352,7 +13448,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
         <v>144</v>
       </c>
@@ -13369,7 +13465,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
         <v>144</v>
       </c>
@@ -13386,7 +13482,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
         <v>144</v>
       </c>
@@ -13403,7 +13499,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="289" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
         <v>144</v>
       </c>
@@ -13420,7 +13516,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="290" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
         <v>144</v>
       </c>
@@ -13437,7 +13533,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="291" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
         <v>144</v>
       </c>
@@ -13454,7 +13550,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="292" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
         <v>144</v>
       </c>
@@ -13471,7 +13567,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="293" s="11" customFormat="true" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="11" t="s">
         <v>144</v>
       </c>
@@ -13488,7 +13584,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="294" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="294" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="11" t="s">
         <v>144</v>
       </c>
@@ -13505,7 +13601,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="295" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="11" t="s">
         <v>144</v>
       </c>
@@ -13522,7 +13618,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="11" t="s">
         <v>144</v>
       </c>
@@ -13539,7 +13635,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="11" t="s">
         <v>144</v>
       </c>
@@ -13556,7 +13652,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="11" t="s">
         <v>144</v>
       </c>
@@ -13573,7 +13669,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="11" t="s">
         <v>144</v>
       </c>
@@ -13590,7 +13686,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="11" t="s">
         <v>144</v>
       </c>
@@ -13607,7 +13703,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="301" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="11" t="s">
         <v>144</v>
       </c>
@@ -13624,7 +13720,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="11" t="s">
         <v>144</v>
       </c>
@@ -13641,7 +13737,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="303" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="11" t="s">
         <v>144</v>
       </c>
@@ -13658,7 +13754,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="304" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="11" t="s">
         <v>144</v>
       </c>
@@ -13675,7 +13771,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="305" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="11" t="s">
         <v>144</v>
       </c>
@@ -13692,7 +13788,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="11" t="s">
         <v>144</v>
       </c>
@@ -13709,7 +13805,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="307" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="11" t="s">
         <v>144</v>
       </c>
@@ -13726,7 +13822,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="308" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="11" t="s">
         <v>144</v>
       </c>
@@ -13743,7 +13839,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="309" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="11" t="s">
         <v>144</v>
       </c>
@@ -13760,7 +13856,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="310" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="11" t="s">
         <v>144</v>
       </c>
@@ -13777,7 +13873,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="311" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="11" t="s">
         <v>144</v>
       </c>
@@ -13794,7 +13890,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="11" t="s">
         <v>144</v>
       </c>
@@ -13811,7 +13907,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="313" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="11" t="s">
         <v>144</v>
       </c>
@@ -13828,7 +13924,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="314" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
         <v>144</v>
       </c>
@@ -13845,7 +13941,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="315" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="s">
         <v>144</v>
       </c>
@@ -13862,7 +13958,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="316" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="316" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="s">
         <v>144</v>
       </c>
@@ -13879,7 +13975,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="317" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="s">
         <v>144</v>
       </c>
@@ -13896,7 +13992,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="318" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="s">
         <v>144</v>
       </c>
@@ -13913,7 +14009,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="319" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="319" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="s">
         <v>144</v>
       </c>
@@ -13930,7 +14026,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="320" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="s">
         <v>144</v>
       </c>
@@ -13947,7 +14043,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="321" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="321" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="s">
         <v>144</v>
       </c>
@@ -13964,7 +14060,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="322" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="322" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="s">
         <v>144</v>
       </c>
@@ -13981,7 +14077,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="323" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="323" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0" t="s">
         <v>144</v>
       </c>
@@ -13998,7 +14094,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="324" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="324" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="s">
         <v>144</v>
       </c>
@@ -14015,7 +14111,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="325" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="325" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="s">
         <v>144</v>
       </c>
@@ -14032,7 +14128,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="326" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="0" t="s">
         <v>144</v>
       </c>
@@ -14049,7 +14145,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="327" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="0" t="s">
         <v>144</v>
       </c>
@@ -14066,7 +14162,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="328" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="0" t="s">
         <v>144</v>
       </c>
@@ -14083,7 +14179,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="329" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="0" t="s">
         <v>144</v>
       </c>
@@ -14100,7 +14196,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="330" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="0" t="s">
         <v>144</v>
       </c>
@@ -14117,7 +14213,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="331" s="20" customFormat="true" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="20" t="s">
         <v>144</v>
       </c>
@@ -14134,7 +14230,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="332" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="0" t="s">
         <v>144</v>
       </c>
@@ -14151,7 +14247,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="333" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="0" t="s">
         <v>144</v>
       </c>
@@ -14168,7 +14264,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="334" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="0" t="s">
         <v>144</v>
       </c>
@@ -14185,7 +14281,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="335" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="s">
         <v>144</v>
       </c>
@@ -14202,7 +14298,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="336" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="0" t="s">
         <v>144</v>
       </c>
@@ -14219,7 +14315,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="337" s="20" customFormat="true" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="20" t="s">
         <v>144</v>
       </c>
@@ -14236,7 +14332,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="338" s="11" customFormat="true" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="338" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="11" t="s">
         <v>144</v>
       </c>
@@ -14253,7 +14349,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="339" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="11" t="s">
         <v>144</v>
       </c>
@@ -14270,7 +14366,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="340" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="11" t="s">
         <v>144</v>
       </c>
@@ -14287,7 +14383,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="341" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="11" t="s">
         <v>144</v>
       </c>
@@ -14304,7 +14400,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="342" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="0" t="s">
         <v>144</v>
       </c>
@@ -14321,7 +14417,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="343" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="0" t="s">
         <v>144</v>
       </c>
@@ -14338,7 +14434,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="344" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="0" t="s">
         <v>144</v>
       </c>
@@ -14355,7 +14451,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="345" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="0" t="s">
         <v>144</v>
       </c>
@@ -14372,7 +14468,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="346" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="0" t="s">
         <v>144</v>
       </c>
@@ -14389,7 +14485,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="347" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="0" t="s">
         <v>144</v>
       </c>
@@ -14406,7 +14502,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="348" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="0" t="s">
         <v>144</v>
       </c>
@@ -14423,7 +14519,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="349" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="0" t="s">
         <v>144</v>
       </c>
@@ -14440,7 +14536,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="350" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="0" t="s">
         <v>144</v>
       </c>
@@ -14457,7 +14553,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="351" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="351" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="0" t="s">
         <v>144</v>
       </c>
@@ -14474,7 +14570,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="352" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="0" t="s">
         <v>144</v>
       </c>
@@ -14491,7 +14587,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="353" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="0" t="s">
         <v>144</v>
       </c>
@@ -14508,7 +14604,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="354" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="0" t="s">
         <v>144</v>
       </c>
@@ -14525,7 +14621,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="355" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="0" t="s">
         <v>144</v>
       </c>
@@ -14542,7 +14638,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="356" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="0" t="s">
         <v>144</v>
       </c>
@@ -14559,7 +14655,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="357" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="0" t="s">
         <v>144</v>
       </c>
@@ -14576,7 +14672,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="358" s="11" customFormat="true" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="358" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="11" t="s">
         <v>144</v>
       </c>
@@ -14593,7 +14689,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="359" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="11" t="s">
         <v>144</v>
       </c>
@@ -14610,7 +14706,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="360" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="11" t="s">
         <v>144</v>
       </c>
@@ -14627,7 +14723,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="361" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="11" t="s">
         <v>144</v>
       </c>
@@ -14644,7 +14740,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="362" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="0" t="s">
         <v>139</v>
       </c>
@@ -14661,7 +14757,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="363" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="11" t="s">
         <v>146</v>
       </c>
@@ -14678,7 +14774,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="11" t="s">
         <v>127</v>
       </c>
@@ -14695,7 +14791,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="365" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="11" t="s">
         <v>144</v>
       </c>
@@ -14712,7 +14808,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="366" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="11" t="s">
         <v>144</v>
       </c>
@@ -14729,7 +14825,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="367" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="11" t="s">
         <v>144</v>
       </c>
@@ -14746,7 +14842,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="368" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="11" t="s">
         <v>144</v>
       </c>
@@ -15375,7 +15471,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="405" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="11" t="s">
         <v>127</v>
       </c>
@@ -15392,7 +15488,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="406" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="11" t="s">
         <v>127</v>
       </c>
@@ -15409,7 +15505,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="407" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="11" t="s">
         <v>146</v>
       </c>
@@ -15426,7 +15522,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="408" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="11" t="s">
         <v>146</v>
       </c>
@@ -15443,7 +15539,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="409" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="0" t="s">
         <v>139</v>
       </c>
@@ -15460,7 +15556,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="410" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="0" t="s">
         <v>139</v>
       </c>
@@ -15477,7 +15573,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="411" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="411" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="0" t="s">
         <v>144</v>
       </c>
@@ -15494,7 +15590,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="412" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="412" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="0" t="s">
         <v>144</v>
       </c>
@@ -15511,7 +15607,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="413" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="413" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="0" t="s">
         <v>144</v>
       </c>
@@ -15528,7 +15624,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="414" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="414" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="0" t="s">
         <v>144</v>
       </c>
@@ -15545,7 +15641,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="415" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="415" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="0" t="s">
         <v>144</v>
       </c>
@@ -15562,7 +15658,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="416" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="416" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="0" t="s">
         <v>144</v>
       </c>
@@ -15579,7 +15675,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="417" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="11" t="s">
         <v>127</v>
       </c>
@@ -15596,7 +15692,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="418" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="11" t="s">
         <v>127</v>
       </c>
@@ -15613,7 +15709,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="419" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="11" t="s">
         <v>127</v>
       </c>
@@ -15630,7 +15726,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="420" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="11" t="s">
         <v>127</v>
       </c>
@@ -15647,7 +15743,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="421" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="11" t="s">
         <v>127</v>
       </c>
@@ -15664,7 +15760,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="422" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="11" t="s">
         <v>127</v>
       </c>
@@ -15681,7 +15777,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="423" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="11" t="s">
         <v>146</v>
       </c>
@@ -15698,7 +15794,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="424" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="11" t="s">
         <v>146</v>
       </c>
@@ -15715,7 +15811,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="425" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="11" t="s">
         <v>146</v>
       </c>
@@ -15732,7 +15828,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="426" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="11" t="s">
         <v>146</v>
       </c>
@@ -15749,7 +15845,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="427" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="11" t="s">
         <v>146</v>
       </c>
@@ -15766,7 +15862,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="428" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="11" t="s">
         <v>146</v>
       </c>
@@ -15783,7 +15879,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="429" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="0" t="s">
         <v>139</v>
       </c>
@@ -15800,7 +15896,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="430" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="0" t="s">
         <v>139</v>
       </c>
@@ -15817,7 +15913,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="431" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="0" t="s">
         <v>139</v>
       </c>
@@ -15834,7 +15930,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="432" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="0" t="s">
         <v>139</v>
       </c>
@@ -15851,7 +15947,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="433" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="0" t="s">
         <v>139</v>
       </c>
@@ -15868,7 +15964,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="434" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="0" t="s">
         <v>139</v>
       </c>
@@ -15885,7 +15981,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="435" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="11" t="s">
         <v>146</v>
       </c>
@@ -15902,7 +15998,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="436" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="0" t="s">
         <v>139</v>
       </c>
@@ -15919,7 +16015,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="437" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="11" t="s">
         <v>127</v>
       </c>
@@ -15936,7 +16032,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="438" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="438" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="0" t="s">
         <v>144</v>
       </c>
@@ -15953,7 +16049,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="439" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="439" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="0" t="s">
         <v>144</v>
       </c>
@@ -15970,7 +16066,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="440" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="440" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="0" t="s">
         <v>144</v>
       </c>
@@ -15989,13 +16085,7 @@
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:F440">
-    <filterColumn colId="4">
-      <customFilters and="true">
-        <customFilter operator="equal" val="anchor"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F440"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
FEM Care orchestration CR
</commit_message>
<xml_diff>
--- a/Projects/PNGAMERICA/Data/Template_v4.4.xlsx
+++ b/Projects/PNGAMERICA/Data/Template_v4.4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="block and availability" sheetId="1" state="visible" r:id="rId2"/>
@@ -47,6 +47,9 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
@@ -62,6 +65,9 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="dfg" vbProcedure="false">main!$A$1:$F$194</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="qwe" vbProcedure="false">main!$A$1:$F$194</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="sdf" vbProcedure="false">main!$A$1:$F$211</definedName>
@@ -94,17 +100,20 @@
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">main!$A$1:$F$440</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">main!$A$1:$F$434</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$434</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$368</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$368</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -670,7 +679,7 @@
     <t>filter attribute 2</t>
   </si>
   <si>
-    <t>ECONOMY, PREMIUM, SUPER PREMIUM</t>
+    <t>ECONOMY, MID TIER, PREMIUM</t>
   </si>
   <si>
     <t>top, bottom</t>
@@ -1491,13 +1500,14 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1581,13 +1591,13 @@
   </sheetPr>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O11" activeCellId="0" sqref="O11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="101.975708502024"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.655870445344"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1626,7 +1636,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
         <v>152</v>
       </c>
@@ -1885,7 +1895,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="74.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.9473684210526"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -2160,8 +2170,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="91.0526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.914979757085"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -2635,8 +2645,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="84.6234817813765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.3765182186235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="86.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.3036437246964"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -3816,7 +3826,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="102.19028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.87044534413"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -5929,8 +5939,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.3481781376518"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.6315789473684"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
@@ -8019,12 +8029,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.0566801619433"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.7692307692308"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -8592,10 +8602,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="100.797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="68.8785425101215"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="103.582995951417"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="70.7004048582996"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>

</xml_diff>

<commit_message>
FEM Care orchestration CR - template fix
</commit_message>
<xml_diff>
--- a/Projects/PNGAMERICA/Data/Template_v4.4.xlsx
+++ b/Projects/PNGAMERICA/Data/Template_v4.4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="block and availability" sheetId="1" state="visible" r:id="rId2"/>
@@ -50,6 +50,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
@@ -68,6 +69,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="dfg" vbProcedure="false">main!$A$1:$F$194</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="qwe" vbProcedure="false">main!$A$1:$F$194</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="sdf" vbProcedure="false">main!$A$1:$F$211</definedName>
@@ -103,17 +105,18 @@
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$434</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$434</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$368</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$368</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -125,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4220" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4220" uniqueCount="223">
   <si>
     <t>kpi Name</t>
   </si>
@@ -689,9 +692,6 @@
   </si>
   <si>
     <t>PADS</t>
-  </si>
-  <si>
-    <t>y</t>
   </si>
   <si>
     <t>TAMPAX</t>
@@ -1194,7 +1194,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="G3 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1289,7 +1289,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="G3 C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1500,13 +1500,13 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="G3 E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="77.5546558704454"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1591,13 +1591,13 @@
   </sheetPr>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.655870445344"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="105.619433198381"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1688,7 +1688,7 @@
         <v>39</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>188</v>
+        <v>39</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>186</v>
@@ -1723,13 +1723,13 @@
         <v>39</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K4" s="0" t="s">
         <v>26</v>
@@ -1758,13 +1758,13 @@
         <v>39</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>26</v>
@@ -1778,13 +1778,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>192</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,13 +1795,13 @@
         <v>29</v>
       </c>
       <c r="C7" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>195</v>
-      </c>
       <c r="E7" s="0" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -1823,7 +1823,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="G3 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1868,7 +1868,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1890,12 +1890,12 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="1" sqref="G3 I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.9473684210526"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.6963562753036"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1904,55 +1904,55 @@
         <v>16</v>
       </c>
       <c r="B1" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="I1" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="J1" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="L1" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="M1" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="N1" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="O1" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="P1" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="Q1" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="R1" s="0" t="s">
         <v>211</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1963,37 +1963,37 @@
         <v>26</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>216</v>
-      </c>
       <c r="H2" s="0" t="s">
         <v>26</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>22</v>
       </c>
       <c r="K2" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="L2" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="L2" s="0" t="s">
-        <v>215</v>
-      </c>
       <c r="M2" s="0" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P2" s="0" t="n">
         <v>1</v>
@@ -2010,14 +2010,14 @@
         <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D3" s="28"/>
       <c r="H3" s="28" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N3" s="28" t="n">
         <v>1</v>
@@ -2037,13 +2037,13 @@
         <v>26</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>220</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>221</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>1</v>
@@ -2069,10 +2069,10 @@
         <v>7</v>
       </c>
       <c r="H5" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="I5" s="0" t="s">
         <v>222</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>223</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>1</v>
@@ -2106,7 +2106,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="G3 A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2165,13 +2165,13 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="1" sqref="G3 A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="93.4089068825911"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.2631578947368"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -2640,13 +2640,13 @@
   <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
+      <selection pane="topLeft" activeCell="B64" activeCellId="1" sqref="G3 B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="86.8744939271255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.3036437246964"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="87.6234817813765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.9473684210526"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -3821,12 +3821,12 @@
   <dimension ref="A1:K122"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="1" sqref="G3 C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.87044534413"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="105.834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -5934,13 +5934,13 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H35" activeCellId="0" sqref="H35"/>
+      <selection pane="topLeft" activeCell="H35" activeCellId="1" sqref="G3 H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.6315789473684"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6356275303644"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
@@ -7036,7 +7036,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="G3 B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7311,7 +7311,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G37" activeCellId="0" sqref="G37"/>
+      <selection pane="topLeft" activeCell="G37" activeCellId="1" sqref="G3 G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8024,17 +8024,17 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
+      <selection pane="topLeft" activeCell="A44" activeCellId="1" sqref="G3 A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.7692307692308"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="66.3076923076923"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6356275303644"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -8596,16 +8596,16 @@
   <dimension ref="A1:F441"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A349" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B375" activeCellId="0" sqref="B375"/>
+      <selection pane="topLeft" activeCell="B375" activeCellId="1" sqref="G3 B375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="103.582995951417"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="70.7004048582996"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="104.441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.2348178137652"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>

</xml_diff>

<commit_message>
Number of shelves for all categories + AI Eye Level fix
</commit_message>
<xml_diff>
--- a/Projects/PNGAMERICA/Data/Template_v4.4.xlsx
+++ b/Projects/PNGAMERICA/Data/Template_v4.4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="block and availability" sheetId="1" state="visible" r:id="rId2"/>
@@ -51,6 +51,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
@@ -70,6 +71,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="dfg" vbProcedure="false">main!$A$1:$F$194</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="qwe" vbProcedure="false">main!$A$1:$F$194</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="sdf" vbProcedure="false">main!$A$1:$F$211</definedName>
@@ -106,17 +108,18 @@
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$434</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$434</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$368</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$368</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -128,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4220" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4241" uniqueCount="223">
   <si>
     <t>kpi Name</t>
   </si>
@@ -1194,7 +1197,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="G3 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1289,7 +1292,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="G3 C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1501,12 +1504,12 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="G3 E5"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="77.5546558704454"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="78.1983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1591,13 +1594,13 @@
   </sheetPr>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="105.619433198381"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="106.582995951417"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1823,7 +1826,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="G3 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1890,12 +1893,12 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="1" sqref="G3 I3"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.6963562753036"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="77.3400809716599"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -2103,15 +2106,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="G3 A18"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.0931174089069"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2144,6 +2148,30 @@
       </c>
       <c r="B4" s="0" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2165,13 +2193,13 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="1" sqref="G3 A32"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.2631578947368"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="95.0161943319838"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.4858299595142"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -2640,13 +2668,13 @@
   <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B64" activeCellId="1" sqref="G3 B64"/>
+      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="87.6234817813765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.9473684210526"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="88.4817813765182"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="76.6963562753036"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -3821,12 +3849,12 @@
   <dimension ref="A1:K122"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="1" sqref="G3 C21"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="105.834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="106.692307692308"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -5934,13 +5962,13 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H35" activeCellId="1" sqref="G3 H35"/>
+      <selection pane="topLeft" activeCell="H35" activeCellId="0" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.0607287449393"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.4898785425101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
@@ -7036,7 +7064,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="G3 B11"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7311,7 +7339,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G37" activeCellId="1" sqref="G3 G37"/>
+      <selection pane="topLeft" activeCell="G37" activeCellId="0" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8024,17 +8052,17 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A44" activeCellId="1" sqref="G3 A44"/>
+      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="66.3076923076923"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="66.9473684210526"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -8593,19 +8621,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F441"/>
+  <dimension ref="A1:F443"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A349" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B375" activeCellId="1" sqref="G3 B375"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C427" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E449" activeCellId="0" sqref="E449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="104.441295546559"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.2348178137652"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="105.404858299595"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.8785425101215"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
@@ -16093,7 +16121,57 @@
         <v>129</v>
       </c>
     </row>
-    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A441" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B441" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C441" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D441" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E441" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A442" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B442" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C442" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D442" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E442" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A443" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B443" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C443" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D443" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E443" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F440"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
running relative and shelves in addition to OSA
</commit_message>
<xml_diff>
--- a/Projects/PNGAMERICA/Data/Template_v4.4.xlsx
+++ b/Projects/PNGAMERICA/Data/Template_v4.4.xlsx
@@ -27,7 +27,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
-    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$440</definedName>
+    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$442</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
@@ -52,6 +52,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
@@ -72,54 +73,56 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="dfg" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="qwe" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="sdf" vbProcedure="false">main!$A$1:$F$211</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="wqe" vbProcedure="false">main!$A$1:$F$211</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0" vbProcedure="false">main!$A$1:$F$358</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0" vbProcedure="false">main!$A$1:$F$358</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0" vbProcedure="false">main!$A$1:$F$358</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0" vbProcedure="false">main!$A$1:$F$358</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$211</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$211</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$211</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$211</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$211</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$211</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$211</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$211</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$194</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$440</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">main!$A$1:$F$440</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$440</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$434</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$416</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$404</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$368</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'anchor new'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="dfg" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="qwe" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="sdf" vbProcedure="false">main!$A$1:$F$210</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="wqe" vbProcedure="false">main!$A$1:$F$210</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$210</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$210</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$210</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$210</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$210</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$210</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$210</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$210</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$193</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$439</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">main!$A$1:$F$439</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">main!$A$1:$F$439</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">main!$A$1:$F$439</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">main!$A$1:$F$439</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$439</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$439</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$439</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$439</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$439</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$433</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$415</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$415</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$415</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$403</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$415</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$403</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$403</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$403</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$403</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$367</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -604,40 +607,40 @@
     <t>Orchestration:Tampax_Orchest_2:FEM CARE</t>
   </si>
   <si>
+    <t>block and availability</t>
+  </si>
+  <si>
+    <t>Adjacency:One_Brush_Adj:ORAL CARE</t>
+  </si>
+  <si>
+    <t>Shelves:Num_of_Shleves:{category}</t>
+  </si>
+  <si>
+    <t>average shelf</t>
+  </si>
+  <si>
+    <t>Orchestration:Absorbency_Orchestration:FEM CARE</t>
+  </si>
+  <si>
+    <t>Orchestration:Absorbency_Orchestration:AI</t>
+  </si>
+  <si>
+    <t>Adjacency:Naturals Adjacency:FABRICARE:NATURALS=GREEN:BENEFIT=FREE/SENSITIVE</t>
+  </si>
+  <si>
+    <t>Orchestration:SUD_Horiz_Orches:FABRICARE:SEG=LAUNDRY CARE:FORM=LAUNDRY UNIT DOSE</t>
+  </si>
+  <si>
+    <t>sud_orchestration</t>
+  </si>
+  <si>
+    <t>Blocking:Regimen_Presence:FABRIC_CARE</t>
+  </si>
+  <si>
+    <t>fabricare_regimen</t>
+  </si>
+  <si>
     <t>Adjacency:Tide Simply Adjacency:FABRICARE</t>
-  </si>
-  <si>
-    <t>block and availability</t>
-  </si>
-  <si>
-    <t>Adjacency:One_Brush_Adj:ORAL CARE</t>
-  </si>
-  <si>
-    <t>Shelves:Num_of_Shleves:{category}</t>
-  </si>
-  <si>
-    <t>average shelf</t>
-  </si>
-  <si>
-    <t>Orchestration:Absorbency_Orchestration:FEM CARE</t>
-  </si>
-  <si>
-    <t>Orchestration:Absorbency_Orchestration:AI</t>
-  </si>
-  <si>
-    <t>Adjacency:Naturals Adjacency:FABRICARE:NATURALS=GREEN:BENEFIT=FREE/SENSITIVE</t>
-  </si>
-  <si>
-    <t>Orchestration:SUD_Horiz_Orches:FABRICARE:SEG=LAUNDRY CARE:FORM=LAUNDRY UNIT DOSE</t>
-  </si>
-  <si>
-    <t>sud_orchestration</t>
-  </si>
-  <si>
-    <t>Blocking:Regimen_Presence:FABRIC_CARE</t>
-  </si>
-  <si>
-    <t>fabricare_regimen</t>
   </si>
   <si>
     <t>brand_list</t>
@@ -1509,7 +1512,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="78.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="78.9473684210526"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1600,7 +1603,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="106.582995951417"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="107.546558704453"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1775,7 +1778,7 @@
     </row>
     <row r="6" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>21</v>
@@ -1792,7 +1795,7 @@
     </row>
     <row r="7" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>29</v>
@@ -1898,7 +1901,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="77.3400809716599"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="77.9838056680162"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -2007,7 +2010,7 @@
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="B3" s="28" t="s">
         <v>22</v>
@@ -2034,7 +2037,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>26</v>
@@ -2063,7 +2066,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>6</v>
@@ -2114,7 +2117,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.0931174089069"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.663967611336"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -2128,7 +2131,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>31</v>
@@ -2136,7 +2139,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>32</v>
@@ -2144,7 +2147,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>33</v>
@@ -2152,7 +2155,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>30</v>
@@ -2160,7 +2163,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>21</v>
@@ -2168,7 +2171,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>29</v>
@@ -2198,8 +2201,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="95.0161943319838"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.4858299595142"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="95.8704453441296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.914979757085"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -2673,8 +2676,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="88.4817813765182"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="76.6963562753036"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="89.2307692307692"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="77.3400809716599"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -3854,7 +3857,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="106.692307692308"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="107.655870445344"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -5967,8 +5970,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.4898785425101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8097165991903"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.17004048583"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
@@ -8057,12 +8060,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="66.9473684210526"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.5910931174089"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.17004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -8623,17 +8626,17 @@
   </sheetPr>
   <dimension ref="A1:F443"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C427" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E449" activeCellId="0" sqref="E449"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A130" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B149" activeCellId="0" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="105.404858299595"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.8785425101215"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="106.368421052632"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="72.5182186234818"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
@@ -11243,20 +11246,20 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="0" t="s">
-        <v>144</v>
+      <c r="A154" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>157</v>
+        <v>76</v>
       </c>
       <c r="C154" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="D154" s="15" t="s">
-        <v>145</v>
+        <v>21</v>
+      </c>
+      <c r="D154" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="E154" s="0" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11264,7 +11267,7 @@
         <v>127</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C155" s="11" t="s">
         <v>21</v>
@@ -11281,7 +11284,7 @@
         <v>127</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C156" s="11" t="s">
         <v>21</v>
@@ -11298,7 +11301,7 @@
         <v>127</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C157" s="11" t="s">
         <v>21</v>
@@ -11315,7 +11318,7 @@
         <v>127</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C158" s="11" t="s">
         <v>21</v>
@@ -11332,7 +11335,7 @@
         <v>127</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C159" s="11" t="s">
         <v>21</v>
@@ -11349,7 +11352,7 @@
         <v>127</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="C160" s="11" t="s">
         <v>21</v>
@@ -11357,8 +11360,8 @@
       <c r="D160" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="E160" s="0" t="s">
-        <v>77</v>
+      <c r="E160" s="16" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11366,7 +11369,7 @@
         <v>127</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C161" s="11" t="s">
         <v>21</v>
@@ -11383,7 +11386,7 @@
         <v>127</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C162" s="11" t="s">
         <v>21</v>
@@ -11400,7 +11403,7 @@
         <v>127</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C163" s="11" t="s">
         <v>21</v>
@@ -11417,7 +11420,7 @@
         <v>127</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C164" s="11" t="s">
         <v>21</v>
@@ -11431,13 +11434,13 @@
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="11" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C165" s="11" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D165" s="11" t="s">
         <v>128</v>
@@ -11451,7 +11454,7 @@
         <v>146</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C166" s="11" t="s">
         <v>29</v>
@@ -11468,7 +11471,7 @@
         <v>146</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C167" s="11" t="s">
         <v>29</v>
@@ -11485,7 +11488,7 @@
         <v>146</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C168" s="11" t="s">
         <v>29</v>
@@ -11502,7 +11505,7 @@
         <v>146</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C169" s="11" t="s">
         <v>29</v>
@@ -11515,17 +11518,17 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="11" t="s">
-        <v>146</v>
+      <c r="A170" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C170" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D170" s="11" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="E170" s="16" t="s">
         <v>130</v>
@@ -11536,7 +11539,7 @@
         <v>139</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C171" s="11" t="s">
         <v>30</v>
@@ -11553,7 +11556,7 @@
         <v>139</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C172" s="11" t="s">
         <v>30</v>
@@ -11570,7 +11573,7 @@
         <v>139</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C173" s="11" t="s">
         <v>30</v>
@@ -11587,7 +11590,7 @@
         <v>139</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C174" s="11" t="s">
         <v>30</v>
@@ -11601,16 +11604,16 @@
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C175" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D175" s="11" t="s">
-        <v>141</v>
+        <v>31</v>
+      </c>
+      <c r="D175" s="15" t="s">
+        <v>145</v>
       </c>
       <c r="E175" s="16" t="s">
         <v>130</v>
@@ -11621,7 +11624,7 @@
         <v>144</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C176" s="11" t="s">
         <v>31</v>
@@ -11638,7 +11641,7 @@
         <v>144</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C177" s="11" t="s">
         <v>31</v>
@@ -11655,7 +11658,7 @@
         <v>144</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C178" s="11" t="s">
         <v>31</v>
@@ -11672,7 +11675,7 @@
         <v>144</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C179" s="11" t="s">
         <v>31</v>
@@ -11686,19 +11689,19 @@
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="C180" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D180" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E180" s="16" t="s">
-        <v>130</v>
+        <v>30</v>
+      </c>
+      <c r="D180" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E180" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11706,7 +11709,7 @@
         <v>139</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C181" s="11" t="s">
         <v>30</v>
@@ -11723,7 +11726,7 @@
         <v>139</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C182" s="11" t="s">
         <v>30</v>
@@ -11740,7 +11743,7 @@
         <v>139</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C183" s="11" t="s">
         <v>30</v>
@@ -11757,7 +11760,7 @@
         <v>139</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C184" s="11" t="s">
         <v>30</v>
@@ -11774,7 +11777,7 @@
         <v>139</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C185" s="11" t="s">
         <v>30</v>
@@ -11791,7 +11794,7 @@
         <v>139</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C186" s="11" t="s">
         <v>30</v>
@@ -11808,7 +11811,7 @@
         <v>139</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C187" s="11" t="s">
         <v>30</v>
@@ -11825,7 +11828,7 @@
         <v>139</v>
       </c>
       <c r="B188" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C188" s="11" t="s">
         <v>30</v>
@@ -11842,7 +11845,7 @@
         <v>139</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C189" s="11" t="s">
         <v>30</v>
@@ -11859,7 +11862,7 @@
         <v>139</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C190" s="11" t="s">
         <v>30</v>
@@ -11876,7 +11879,7 @@
         <v>139</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C191" s="11" t="s">
         <v>30</v>
@@ -11893,7 +11896,7 @@
         <v>139</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="C192" s="11" t="s">
         <v>30</v>
@@ -11901,8 +11904,8 @@
       <c r="D192" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="E192" s="0" t="s">
-        <v>131</v>
+      <c r="E192" s="11" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11910,7 +11913,7 @@
         <v>139</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C193" s="11" t="s">
         <v>30</v>
@@ -11924,27 +11927,27 @@
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="C194" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D194" s="11" t="s">
-        <v>141</v>
+        <v>147</v>
+      </c>
+      <c r="D194" s="15" t="s">
+        <v>145</v>
       </c>
       <c r="E194" s="11" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B195" s="0" t="s">
-        <v>103</v>
+      <c r="B195" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="C195" s="11" t="s">
         <v>147</v>
@@ -11960,8 +11963,8 @@
       <c r="A196" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B196" s="11" t="s">
-        <v>104</v>
+      <c r="B196" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="C196" s="11" t="s">
         <v>147</v>
@@ -11978,7 +11981,7 @@
         <v>144</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="C197" s="11" t="s">
         <v>147</v>
@@ -11987,24 +11990,24 @@
         <v>145</v>
       </c>
       <c r="E197" s="11" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="C198" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="D198" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E198" s="11" t="s">
-        <v>158</v>
+        <v>30</v>
+      </c>
+      <c r="D198" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E198" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12012,7 +12015,7 @@
         <v>139</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C199" s="11" t="s">
         <v>30</v>
@@ -12029,7 +12032,7 @@
         <v>139</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C200" s="11" t="s">
         <v>30</v>
@@ -12046,7 +12049,7 @@
         <v>139</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C201" s="11" t="s">
         <v>30</v>
@@ -12063,7 +12066,7 @@
         <v>139</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C202" s="11" t="s">
         <v>30</v>
@@ -12080,7 +12083,7 @@
         <v>139</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C203" s="11" t="s">
         <v>30</v>
@@ -12093,17 +12096,17 @@
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="0" t="s">
-        <v>139</v>
+      <c r="A204" s="11" t="s">
+        <v>146</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C204" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D204" s="11" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="E204" s="0" t="s">
         <v>77</v>
@@ -12114,7 +12117,7 @@
         <v>146</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C205" s="11" t="s">
         <v>29</v>
@@ -12131,7 +12134,7 @@
         <v>146</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C206" s="11" t="s">
         <v>29</v>
@@ -12148,7 +12151,7 @@
         <v>146</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C207" s="11" t="s">
         <v>29</v>
@@ -12165,7 +12168,7 @@
         <v>146</v>
       </c>
       <c r="B208" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C208" s="11" t="s">
         <v>29</v>
@@ -12182,7 +12185,7 @@
         <v>146</v>
       </c>
       <c r="B209" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C209" s="11" t="s">
         <v>29</v>
@@ -12195,20 +12198,20 @@
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="11" t="s">
-        <v>146</v>
+      <c r="A210" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="B210" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C210" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D210" s="11" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="E210" s="0" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12216,7 +12219,7 @@
         <v>139</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>83</v>
+        <v>158</v>
       </c>
       <c r="C211" s="11" t="s">
         <v>30</v>
@@ -12225,32 +12228,32 @@
         <v>141</v>
       </c>
       <c r="E211" s="0" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>159</v>
+        <v>103</v>
       </c>
       <c r="C212" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D212" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="E212" s="0" t="s">
-        <v>151</v>
+        <v>31</v>
+      </c>
+      <c r="D212" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E212" s="11" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B213" s="0" t="s">
-        <v>103</v>
+      <c r="B213" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="C213" s="11" t="s">
         <v>31</v>
@@ -12266,8 +12269,8 @@
       <c r="A214" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B214" s="11" t="s">
-        <v>104</v>
+      <c r="B214" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="C214" s="11" t="s">
         <v>31</v>
@@ -12284,10 +12287,10 @@
         <v>144</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C215" s="11" t="s">
-        <v>31</v>
+        <v>103</v>
+      </c>
+      <c r="C215" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="D215" s="15" t="s">
         <v>145</v>
@@ -12300,8 +12303,8 @@
       <c r="A216" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B216" s="0" t="s">
-        <v>103</v>
+      <c r="B216" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="C216" s="0" t="s">
         <v>32</v>
@@ -12317,8 +12320,8 @@
       <c r="A217" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B217" s="11" t="s">
-        <v>104</v>
+      <c r="B217" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="C217" s="0" t="s">
         <v>32</v>
@@ -12335,10 +12338,10 @@
         <v>144</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D218" s="15" t="s">
         <v>145</v>
@@ -12351,8 +12354,8 @@
       <c r="A219" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B219" s="0" t="s">
-        <v>103</v>
+      <c r="B219" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="C219" s="0" t="s">
         <v>33</v>
@@ -12368,8 +12371,8 @@
       <c r="A220" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B220" s="11" t="s">
-        <v>104</v>
+      <c r="B220" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="C220" s="0" t="s">
         <v>33</v>
@@ -12386,16 +12389,16 @@
         <v>144</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C221" s="0" t="s">
-        <v>33</v>
+        <v>159</v>
+      </c>
+      <c r="C221" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="D221" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E221" s="11" t="s">
-        <v>138</v>
+      <c r="E221" s="0" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12403,16 +12406,16 @@
         <v>144</v>
       </c>
       <c r="B222" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C222" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D222" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E222" s="0" t="s">
         <v>160</v>
-      </c>
-      <c r="C222" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D222" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E222" s="0" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12420,44 +12423,44 @@
         <v>144</v>
       </c>
       <c r="B223" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C223" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D223" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E223" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="C223" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D223" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E223" s="0" t="s">
+    </row>
+    <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B224" s="19" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B224" s="0" t="s">
-        <v>160</v>
-      </c>
       <c r="C224" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D224" s="15" t="s">
-        <v>145</v>
+        <v>21</v>
+      </c>
+      <c r="D224" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="E224" s="0" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="11" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B225" s="19" t="s">
         <v>162</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D225" s="11" t="s">
         <v>128</v>
@@ -12467,20 +12470,20 @@
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="B226" s="19" t="s">
-        <v>163</v>
+      <c r="A226" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B226" s="0" t="s">
+        <v>20</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D226" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="E226" s="0" t="s">
-        <v>153</v>
+        <v>32</v>
+      </c>
+      <c r="D226" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E226" s="16" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12488,7 +12491,7 @@
         <v>144</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C227" s="0" t="s">
         <v>32</v>
@@ -12505,7 +12508,7 @@
         <v>144</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C228" s="0" t="s">
         <v>32</v>
@@ -12522,7 +12525,7 @@
         <v>144</v>
       </c>
       <c r="B229" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C229" s="0" t="s">
         <v>32</v>
@@ -12534,12 +12537,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
         <v>144</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C230" s="0" t="s">
         <v>32</v>
@@ -12551,15 +12554,15 @@
         <v>129</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
         <v>144</v>
       </c>
       <c r="B231" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C231" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D231" s="15" t="s">
         <v>145</v>
@@ -12573,7 +12576,7 @@
         <v>144</v>
       </c>
       <c r="B232" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C232" s="0" t="s">
         <v>33</v>
@@ -12590,7 +12593,7 @@
         <v>144</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C233" s="0" t="s">
         <v>33</v>
@@ -12607,7 +12610,7 @@
         <v>144</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C234" s="0" t="s">
         <v>33</v>
@@ -12619,12 +12622,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
         <v>144</v>
       </c>
       <c r="B235" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C235" s="0" t="s">
         <v>33</v>
@@ -12636,21 +12639,21 @@
         <v>129</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
         <v>144</v>
       </c>
       <c r="B236" s="0" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C236" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D236" s="15" t="s">
         <v>145</v>
       </c>
       <c r="E236" s="16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12658,7 +12661,7 @@
         <v>144</v>
       </c>
       <c r="B237" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C237" s="0" t="s">
         <v>32</v>
@@ -12675,7 +12678,7 @@
         <v>144</v>
       </c>
       <c r="B238" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C238" s="0" t="s">
         <v>32</v>
@@ -12692,7 +12695,7 @@
         <v>144</v>
       </c>
       <c r="B239" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C239" s="0" t="s">
         <v>32</v>
@@ -12709,7 +12712,7 @@
         <v>144</v>
       </c>
       <c r="B240" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C240" s="0" t="s">
         <v>32</v>
@@ -12726,10 +12729,10 @@
         <v>144</v>
       </c>
       <c r="B241" s="0" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C241" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D241" s="15" t="s">
         <v>145</v>
@@ -12743,7 +12746,7 @@
         <v>144</v>
       </c>
       <c r="B242" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C242" s="0" t="s">
         <v>33</v>
@@ -12760,7 +12763,7 @@
         <v>144</v>
       </c>
       <c r="B243" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C243" s="0" t="s">
         <v>33</v>
@@ -12777,7 +12780,7 @@
         <v>144</v>
       </c>
       <c r="B244" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C244" s="0" t="s">
         <v>33</v>
@@ -12794,7 +12797,7 @@
         <v>144</v>
       </c>
       <c r="B245" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C245" s="0" t="s">
         <v>33</v>
@@ -12811,10 +12814,10 @@
         <v>144</v>
       </c>
       <c r="B246" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C246" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D246" s="15" t="s">
         <v>145</v>
@@ -12828,7 +12831,7 @@
         <v>144</v>
       </c>
       <c r="B247" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C247" s="0" t="s">
         <v>32</v>
@@ -12845,7 +12848,7 @@
         <v>144</v>
       </c>
       <c r="B248" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C248" s="0" t="s">
         <v>32</v>
@@ -12862,7 +12865,7 @@
         <v>144</v>
       </c>
       <c r="B249" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C249" s="0" t="s">
         <v>32</v>
@@ -12879,7 +12882,7 @@
         <v>144</v>
       </c>
       <c r="B250" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C250" s="0" t="s">
         <v>32</v>
@@ -12896,10 +12899,10 @@
         <v>144</v>
       </c>
       <c r="B251" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C251" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D251" s="15" t="s">
         <v>145</v>
@@ -12913,7 +12916,7 @@
         <v>144</v>
       </c>
       <c r="B252" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C252" s="0" t="s">
         <v>33</v>
@@ -12930,7 +12933,7 @@
         <v>144</v>
       </c>
       <c r="B253" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C253" s="0" t="s">
         <v>33</v>
@@ -12947,7 +12950,7 @@
         <v>144</v>
       </c>
       <c r="B254" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C254" s="0" t="s">
         <v>33</v>
@@ -12964,7 +12967,7 @@
         <v>144</v>
       </c>
       <c r="B255" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C255" s="0" t="s">
         <v>33</v>
@@ -12981,16 +12984,16 @@
         <v>144</v>
       </c>
       <c r="B256" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C256" s="0" t="s">
-        <v>33</v>
+        <v>108</v>
+      </c>
+      <c r="C256" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="D256" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E256" s="16" t="s">
-        <v>130</v>
+      <c r="E256" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12998,7 +13001,7 @@
         <v>144</v>
       </c>
       <c r="B257" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C257" s="11" t="s">
         <v>31</v>
@@ -13015,7 +13018,7 @@
         <v>144</v>
       </c>
       <c r="B258" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C258" s="11" t="s">
         <v>31</v>
@@ -13032,7 +13035,7 @@
         <v>144</v>
       </c>
       <c r="B259" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C259" s="11" t="s">
         <v>31</v>
@@ -13049,7 +13052,7 @@
         <v>144</v>
       </c>
       <c r="B260" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C260" s="11" t="s">
         <v>31</v>
@@ -13066,7 +13069,7 @@
         <v>144</v>
       </c>
       <c r="B261" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C261" s="11" t="s">
         <v>31</v>
@@ -13083,10 +13086,10 @@
         <v>144</v>
       </c>
       <c r="B262" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="C262" s="11" t="s">
-        <v>31</v>
+        <v>108</v>
+      </c>
+      <c r="C262" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="D262" s="15" t="s">
         <v>145</v>
@@ -13100,7 +13103,7 @@
         <v>144</v>
       </c>
       <c r="B263" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C263" s="0" t="s">
         <v>32</v>
@@ -13117,7 +13120,7 @@
         <v>144</v>
       </c>
       <c r="B264" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C264" s="0" t="s">
         <v>32</v>
@@ -13134,7 +13137,7 @@
         <v>144</v>
       </c>
       <c r="B265" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C265" s="0" t="s">
         <v>32</v>
@@ -13151,7 +13154,7 @@
         <v>144</v>
       </c>
       <c r="B266" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C266" s="0" t="s">
         <v>32</v>
@@ -13168,7 +13171,7 @@
         <v>144</v>
       </c>
       <c r="B267" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C267" s="0" t="s">
         <v>32</v>
@@ -13185,10 +13188,10 @@
         <v>144</v>
       </c>
       <c r="B268" s="0" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C268" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D268" s="15" t="s">
         <v>145</v>
@@ -13202,7 +13205,7 @@
         <v>144</v>
       </c>
       <c r="B269" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C269" s="0" t="s">
         <v>33</v>
@@ -13219,7 +13222,7 @@
         <v>144</v>
       </c>
       <c r="B270" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C270" s="0" t="s">
         <v>33</v>
@@ -13236,7 +13239,7 @@
         <v>144</v>
       </c>
       <c r="B271" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C271" s="0" t="s">
         <v>33</v>
@@ -13253,7 +13256,7 @@
         <v>144</v>
       </c>
       <c r="B272" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C272" s="0" t="s">
         <v>33</v>
@@ -13270,7 +13273,7 @@
         <v>144</v>
       </c>
       <c r="B273" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C273" s="0" t="s">
         <v>33</v>
@@ -13282,34 +13285,34 @@
         <v>134</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B274" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="C274" s="0" t="s">
+    <row r="274" s="20" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B274" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C274" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D274" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E274" s="0" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="275" s="20" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="B275" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C275" s="20" t="s">
+      <c r="D274" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="E274" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B275" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C275" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D275" s="21" t="s">
+      <c r="D275" s="15" t="s">
         <v>145</v>
       </c>
       <c r="E275" s="11" t="s">
@@ -13321,7 +13324,7 @@
         <v>144</v>
       </c>
       <c r="B276" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C276" s="11" t="s">
         <v>33</v>
@@ -13338,7 +13341,7 @@
         <v>144</v>
       </c>
       <c r="B277" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C277" s="11" t="s">
         <v>33</v>
@@ -13355,7 +13358,7 @@
         <v>144</v>
       </c>
       <c r="B278" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C278" s="11" t="s">
         <v>33</v>
@@ -13372,7 +13375,7 @@
         <v>144</v>
       </c>
       <c r="B279" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C279" s="11" t="s">
         <v>33</v>
@@ -13389,7 +13392,7 @@
         <v>144</v>
       </c>
       <c r="B280" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C280" s="11" t="s">
         <v>33</v>
@@ -13406,7 +13409,7 @@
         <v>144</v>
       </c>
       <c r="B281" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C281" s="11" t="s">
         <v>33</v>
@@ -13423,7 +13426,7 @@
         <v>144</v>
       </c>
       <c r="B282" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C282" s="11" t="s">
         <v>33</v>
@@ -13440,7 +13443,7 @@
         <v>144</v>
       </c>
       <c r="B283" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C283" s="11" t="s">
         <v>33</v>
@@ -13457,7 +13460,7 @@
         <v>144</v>
       </c>
       <c r="B284" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C284" s="11" t="s">
         <v>33</v>
@@ -13474,7 +13477,7 @@
         <v>144</v>
       </c>
       <c r="B285" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C285" s="11" t="s">
         <v>33</v>
@@ -13491,7 +13494,7 @@
         <v>144</v>
       </c>
       <c r="B286" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C286" s="11" t="s">
         <v>33</v>
@@ -13503,12 +13506,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
         <v>144</v>
       </c>
       <c r="B287" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C287" s="11" t="s">
         <v>33</v>
@@ -13516,8 +13519,8 @@
       <c r="D287" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E287" s="11" t="s">
-        <v>132</v>
+      <c r="E287" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13525,7 +13528,7 @@
         <v>144</v>
       </c>
       <c r="B288" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C288" s="11" t="s">
         <v>33</v>
@@ -13542,7 +13545,7 @@
         <v>144</v>
       </c>
       <c r="B289" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C289" s="11" t="s">
         <v>33</v>
@@ -13559,7 +13562,7 @@
         <v>144</v>
       </c>
       <c r="B290" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C290" s="11" t="s">
         <v>33</v>
@@ -13576,7 +13579,7 @@
         <v>144</v>
       </c>
       <c r="B291" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C291" s="11" t="s">
         <v>33</v>
@@ -13588,12 +13591,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B292" s="0" t="s">
-        <v>81</v>
+    <row r="292" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B292" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="C292" s="11" t="s">
         <v>33</v>
@@ -13601,25 +13604,25 @@
       <c r="D292" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E292" s="0" t="s">
+      <c r="E292" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="293" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B293" s="11" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="C293" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D293" s="15" t="s">
         <v>145</v>
       </c>
       <c r="E293" s="11" t="s">
-        <v>77</v>
+        <v>132</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13627,7 +13630,7 @@
         <v>144</v>
       </c>
       <c r="B294" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C294" s="11" t="s">
         <v>32</v>
@@ -13644,7 +13647,7 @@
         <v>144</v>
       </c>
       <c r="B295" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C295" s="11" t="s">
         <v>32</v>
@@ -13661,7 +13664,7 @@
         <v>144</v>
       </c>
       <c r="B296" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C296" s="11" t="s">
         <v>32</v>
@@ -13678,7 +13681,7 @@
         <v>144</v>
       </c>
       <c r="B297" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C297" s="11" t="s">
         <v>32</v>
@@ -13695,7 +13698,7 @@
         <v>144</v>
       </c>
       <c r="B298" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C298" s="11" t="s">
         <v>32</v>
@@ -13712,7 +13715,7 @@
         <v>144</v>
       </c>
       <c r="B299" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C299" s="11" t="s">
         <v>32</v>
@@ -13729,7 +13732,7 @@
         <v>144</v>
       </c>
       <c r="B300" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C300" s="11" t="s">
         <v>32</v>
@@ -13746,7 +13749,7 @@
         <v>144</v>
       </c>
       <c r="B301" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C301" s="11" t="s">
         <v>32</v>
@@ -13763,7 +13766,7 @@
         <v>144</v>
       </c>
       <c r="B302" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C302" s="11" t="s">
         <v>32</v>
@@ -13780,7 +13783,7 @@
         <v>144</v>
       </c>
       <c r="B303" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C303" s="11" t="s">
         <v>32</v>
@@ -13797,7 +13800,7 @@
         <v>144</v>
       </c>
       <c r="B304" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C304" s="11" t="s">
         <v>32</v>
@@ -13814,7 +13817,7 @@
         <v>144</v>
       </c>
       <c r="B305" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C305" s="11" t="s">
         <v>32</v>
@@ -13826,12 +13829,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B306" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C306" s="11" t="s">
         <v>32</v>
@@ -13840,7 +13843,7 @@
         <v>145</v>
       </c>
       <c r="E306" s="11" t="s">
-        <v>132</v>
+        <v>77</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13848,7 +13851,7 @@
         <v>144</v>
       </c>
       <c r="B307" s="11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C307" s="11" t="s">
         <v>32</v>
@@ -13865,7 +13868,7 @@
         <v>144</v>
       </c>
       <c r="B308" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C308" s="11" t="s">
         <v>32</v>
@@ -13882,7 +13885,7 @@
         <v>144</v>
       </c>
       <c r="B309" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C309" s="11" t="s">
         <v>32</v>
@@ -13899,7 +13902,7 @@
         <v>144</v>
       </c>
       <c r="B310" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C310" s="11" t="s">
         <v>32</v>
@@ -13916,7 +13919,7 @@
         <v>144</v>
       </c>
       <c r="B311" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C311" s="11" t="s">
         <v>32</v>
@@ -13928,29 +13931,29 @@
         <v>77</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B312" s="11" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="C312" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D312" s="15" t="s">
         <v>145</v>
       </c>
       <c r="E312" s="11" t="s">
-        <v>77</v>
+        <v>132</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B313" s="11" t="s">
-        <v>61</v>
+      <c r="A313" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B313" s="0" t="s">
+        <v>63</v>
       </c>
       <c r="C313" s="11" t="s">
         <v>31</v>
@@ -13967,7 +13970,7 @@
         <v>144</v>
       </c>
       <c r="B314" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C314" s="11" t="s">
         <v>31</v>
@@ -13984,7 +13987,7 @@
         <v>144</v>
       </c>
       <c r="B315" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C315" s="11" t="s">
         <v>31</v>
@@ -14001,7 +14004,7 @@
         <v>144</v>
       </c>
       <c r="B316" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C316" s="11" t="s">
         <v>31</v>
@@ -14018,7 +14021,7 @@
         <v>144</v>
       </c>
       <c r="B317" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C317" s="11" t="s">
         <v>31</v>
@@ -14035,7 +14038,7 @@
         <v>144</v>
       </c>
       <c r="B318" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C318" s="11" t="s">
         <v>31</v>
@@ -14052,7 +14055,7 @@
         <v>144</v>
       </c>
       <c r="B319" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C319" s="11" t="s">
         <v>31</v>
@@ -14069,7 +14072,7 @@
         <v>144</v>
       </c>
       <c r="B320" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C320" s="11" t="s">
         <v>31</v>
@@ -14086,7 +14089,7 @@
         <v>144</v>
       </c>
       <c r="B321" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C321" s="11" t="s">
         <v>31</v>
@@ -14103,7 +14106,7 @@
         <v>144</v>
       </c>
       <c r="B322" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C322" s="11" t="s">
         <v>31</v>
@@ -14120,7 +14123,7 @@
         <v>144</v>
       </c>
       <c r="B323" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C323" s="11" t="s">
         <v>31</v>
@@ -14137,7 +14140,7 @@
         <v>144</v>
       </c>
       <c r="B324" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C324" s="11" t="s">
         <v>31</v>
@@ -14149,12 +14152,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="325" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="s">
         <v>144</v>
       </c>
       <c r="B325" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C325" s="11" t="s">
         <v>31</v>
@@ -14162,8 +14165,8 @@
       <c r="D325" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E325" s="11" t="s">
-        <v>132</v>
+      <c r="E325" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14171,7 +14174,7 @@
         <v>144</v>
       </c>
       <c r="B326" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C326" s="11" t="s">
         <v>31</v>
@@ -14188,7 +14191,7 @@
         <v>144</v>
       </c>
       <c r="B327" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C327" s="11" t="s">
         <v>31</v>
@@ -14205,7 +14208,7 @@
         <v>144</v>
       </c>
       <c r="B328" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C328" s="11" t="s">
         <v>31</v>
@@ -14222,7 +14225,7 @@
         <v>144</v>
       </c>
       <c r="B329" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C329" s="11" t="s">
         <v>31</v>
@@ -14234,38 +14237,38 @@
         <v>77</v>
       </c>
     </row>
-    <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A330" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B330" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C330" s="11" t="s">
+    <row r="330" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B330" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C330" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D330" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E330" s="0" t="s">
+      <c r="D330" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="E330" s="20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="331" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A331" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="B331" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C331" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D331" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="E331" s="20" t="s">
-        <v>77</v>
+    <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B331" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C331" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D331" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E331" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14273,7 +14276,7 @@
         <v>144</v>
       </c>
       <c r="B332" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C332" s="11" t="s">
         <v>32</v>
@@ -14290,10 +14293,10 @@
         <v>144</v>
       </c>
       <c r="B333" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C333" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D333" s="15" t="s">
         <v>145</v>
@@ -14307,7 +14310,7 @@
         <v>144</v>
       </c>
       <c r="B334" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C334" s="11" t="s">
         <v>33</v>
@@ -14324,10 +14327,10 @@
         <v>144</v>
       </c>
       <c r="B335" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C335" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D335" s="15" t="s">
         <v>145</v>
@@ -14336,46 +14339,46 @@
         <v>136</v>
       </c>
     </row>
-    <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A336" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B336" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="C336" s="11" t="s">
+    <row r="336" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B336" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C336" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D336" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E336" s="0" t="s">
+      <c r="D336" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="E336" s="20" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="337" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="B337" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="C337" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D337" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="E337" s="20" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="338" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B337" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C337" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D337" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E337" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B338" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C338" s="11" t="s">
         <v>32</v>
@@ -14392,7 +14395,7 @@
         <v>144</v>
       </c>
       <c r="B339" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C339" s="11" t="s">
         <v>32</v>
@@ -14409,7 +14412,7 @@
         <v>144</v>
       </c>
       <c r="B340" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C340" s="11" t="s">
         <v>32</v>
@@ -14422,11 +14425,11 @@
       </c>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="11" t="s">
+      <c r="A341" s="0" t="s">
         <v>144</v>
       </c>
       <c r="B341" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C341" s="11" t="s">
         <v>32</v>
@@ -14443,7 +14446,7 @@
         <v>144</v>
       </c>
       <c r="B342" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C342" s="11" t="s">
         <v>32</v>
@@ -14460,7 +14463,7 @@
         <v>144</v>
       </c>
       <c r="B343" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C343" s="11" t="s">
         <v>32</v>
@@ -14477,10 +14480,10 @@
         <v>144</v>
       </c>
       <c r="B344" s="11" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C344" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D344" s="15" t="s">
         <v>145</v>
@@ -14494,7 +14497,7 @@
         <v>144</v>
       </c>
       <c r="B345" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C345" s="11" t="s">
         <v>33</v>
@@ -14511,7 +14514,7 @@
         <v>144</v>
       </c>
       <c r="B346" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C346" s="11" t="s">
         <v>33</v>
@@ -14528,7 +14531,7 @@
         <v>144</v>
       </c>
       <c r="B347" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C347" s="11" t="s">
         <v>33</v>
@@ -14545,7 +14548,7 @@
         <v>144</v>
       </c>
       <c r="B348" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C348" s="11" t="s">
         <v>33</v>
@@ -14562,7 +14565,7 @@
         <v>144</v>
       </c>
       <c r="B349" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C349" s="11" t="s">
         <v>33</v>
@@ -14579,7 +14582,7 @@
         <v>144</v>
       </c>
       <c r="B350" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C350" s="11" t="s">
         <v>33</v>
@@ -14596,10 +14599,10 @@
         <v>144</v>
       </c>
       <c r="B351" s="11" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C351" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D351" s="15" t="s">
         <v>145</v>
@@ -14613,7 +14616,7 @@
         <v>144</v>
       </c>
       <c r="B352" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C352" s="11" t="s">
         <v>31</v>
@@ -14630,7 +14633,7 @@
         <v>144</v>
       </c>
       <c r="B353" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C353" s="11" t="s">
         <v>31</v>
@@ -14647,7 +14650,7 @@
         <v>144</v>
       </c>
       <c r="B354" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C354" s="11" t="s">
         <v>31</v>
@@ -14664,7 +14667,7 @@
         <v>144</v>
       </c>
       <c r="B355" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C355" s="11" t="s">
         <v>31</v>
@@ -14681,7 +14684,7 @@
         <v>144</v>
       </c>
       <c r="B356" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C356" s="11" t="s">
         <v>31</v>
@@ -14693,12 +14696,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="0" t="s">
+    <row r="357" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B357" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C357" s="11" t="s">
         <v>31</v>
@@ -14710,21 +14713,21 @@
         <v>133</v>
       </c>
     </row>
-    <row r="358" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B358" s="11" t="s">
-        <v>122</v>
+      <c r="B358" s="0" t="s">
+        <v>87</v>
       </c>
       <c r="C358" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D358" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E358" s="11" t="s">
-        <v>133</v>
+      <c r="E358" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14732,10 +14735,10 @@
         <v>144</v>
       </c>
       <c r="B359" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C359" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D359" s="15" t="s">
         <v>145</v>
@@ -14752,7 +14755,7 @@
         <v>88</v>
       </c>
       <c r="C360" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D360" s="15" t="s">
         <v>145</v>
@@ -14762,34 +14765,34 @@
       </c>
     </row>
     <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A361" s="11" t="s">
-        <v>144</v>
+      <c r="A361" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="B361" s="0" t="s">
         <v>88</v>
       </c>
       <c r="C361" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D361" s="15" t="s">
-        <v>145</v>
+        <v>30</v>
+      </c>
+      <c r="D361" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="E361" s="0" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A362" s="0" t="s">
-        <v>139</v>
+      <c r="A362" s="11" t="s">
+        <v>146</v>
       </c>
       <c r="B362" s="0" t="s">
         <v>88</v>
       </c>
       <c r="C362" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D362" s="11" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="E362" s="0" t="s">
         <v>77</v>
@@ -14797,13 +14800,13 @@
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="11" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="B363" s="0" t="s">
         <v>88</v>
       </c>
       <c r="C363" s="11" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D363" s="11" t="s">
         <v>128</v>
@@ -14814,19 +14817,19 @@
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="11" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="B364" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C364" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D364" s="11" t="s">
-        <v>128</v>
+        <v>163</v>
+      </c>
+      <c r="C364" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D364" s="15" t="s">
+        <v>145</v>
       </c>
       <c r="E364" s="0" t="s">
-        <v>77</v>
+        <v>151</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14834,16 +14837,16 @@
         <v>144</v>
       </c>
       <c r="B365" s="0" t="s">
-        <v>164</v>
+        <v>49</v>
       </c>
       <c r="C365" s="0" t="s">
-        <v>147</v>
+        <v>33</v>
       </c>
       <c r="D365" s="15" t="s">
         <v>145</v>
       </c>
       <c r="E365" s="0" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14851,7 +14854,7 @@
         <v>144</v>
       </c>
       <c r="B366" s="0" t="s">
-        <v>49</v>
+        <v>164</v>
       </c>
       <c r="C366" s="0" t="s">
         <v>33</v>
@@ -14859,8 +14862,8 @@
       <c r="D366" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E366" s="0" t="s">
-        <v>130</v>
+      <c r="E366" s="11" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14868,33 +14871,33 @@
         <v>144</v>
       </c>
       <c r="B367" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="C367" s="0" t="s">
-        <v>33</v>
+        <v>166</v>
+      </c>
+      <c r="C367" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="D367" s="15" t="s">
         <v>145</v>
       </c>
       <c r="E367" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A368" s="11" t="s">
+      <c r="A368" s="0" t="s">
         <v>144</v>
       </c>
       <c r="B368" s="0" t="s">
-        <v>167</v>
+        <v>91</v>
       </c>
       <c r="C368" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D368" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E368" s="11" t="s">
-        <v>168</v>
+      <c r="E368" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14902,7 +14905,7 @@
         <v>144</v>
       </c>
       <c r="B369" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C369" s="11" t="s">
         <v>31</v>
@@ -14919,7 +14922,7 @@
         <v>144</v>
       </c>
       <c r="B370" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C370" s="11" t="s">
         <v>31</v>
@@ -14936,7 +14939,7 @@
         <v>144</v>
       </c>
       <c r="B371" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C371" s="11" t="s">
         <v>31</v>
@@ -14953,7 +14956,7 @@
         <v>144</v>
       </c>
       <c r="B372" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C372" s="11" t="s">
         <v>31</v>
@@ -14970,7 +14973,7 @@
         <v>144</v>
       </c>
       <c r="B373" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C373" s="11" t="s">
         <v>31</v>
@@ -14987,7 +14990,7 @@
         <v>144</v>
       </c>
       <c r="B374" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C374" s="11" t="s">
         <v>31</v>
@@ -15004,7 +15007,7 @@
         <v>144</v>
       </c>
       <c r="B375" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C375" s="11" t="s">
         <v>31</v>
@@ -15021,7 +15024,7 @@
         <v>144</v>
       </c>
       <c r="B376" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C376" s="11" t="s">
         <v>31</v>
@@ -15038,7 +15041,7 @@
         <v>144</v>
       </c>
       <c r="B377" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C377" s="11" t="s">
         <v>31</v>
@@ -15055,7 +15058,7 @@
         <v>144</v>
       </c>
       <c r="B378" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C378" s="11" t="s">
         <v>31</v>
@@ -15072,7 +15075,7 @@
         <v>144</v>
       </c>
       <c r="B379" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C379" s="11" t="s">
         <v>31</v>
@@ -15089,10 +15092,10 @@
         <v>144</v>
       </c>
       <c r="B380" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="C380" s="11" t="s">
-        <v>31</v>
+        <v>91</v>
+      </c>
+      <c r="C380" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="D380" s="15" t="s">
         <v>145</v>
@@ -15106,7 +15109,7 @@
         <v>144</v>
       </c>
       <c r="B381" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C381" s="0" t="s">
         <v>32</v>
@@ -15123,7 +15126,7 @@
         <v>144</v>
       </c>
       <c r="B382" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C382" s="0" t="s">
         <v>32</v>
@@ -15140,7 +15143,7 @@
         <v>144</v>
       </c>
       <c r="B383" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C383" s="0" t="s">
         <v>32</v>
@@ -15157,7 +15160,7 @@
         <v>144</v>
       </c>
       <c r="B384" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C384" s="0" t="s">
         <v>32</v>
@@ -15174,7 +15177,7 @@
         <v>144</v>
       </c>
       <c r="B385" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C385" s="0" t="s">
         <v>32</v>
@@ -15191,7 +15194,7 @@
         <v>144</v>
       </c>
       <c r="B386" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C386" s="0" t="s">
         <v>32</v>
@@ -15208,7 +15211,7 @@
         <v>144</v>
       </c>
       <c r="B387" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C387" s="0" t="s">
         <v>32</v>
@@ -15225,7 +15228,7 @@
         <v>144</v>
       </c>
       <c r="B388" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C388" s="0" t="s">
         <v>32</v>
@@ -15242,7 +15245,7 @@
         <v>144</v>
       </c>
       <c r="B389" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C389" s="0" t="s">
         <v>32</v>
@@ -15259,7 +15262,7 @@
         <v>144</v>
       </c>
       <c r="B390" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C390" s="0" t="s">
         <v>32</v>
@@ -15276,7 +15279,7 @@
         <v>144</v>
       </c>
       <c r="B391" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C391" s="0" t="s">
         <v>32</v>
@@ -15293,10 +15296,10 @@
         <v>144</v>
       </c>
       <c r="B392" s="0" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C392" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D392" s="15" t="s">
         <v>145</v>
@@ -15310,7 +15313,7 @@
         <v>144</v>
       </c>
       <c r="B393" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C393" s="0" t="s">
         <v>33</v>
@@ -15327,7 +15330,7 @@
         <v>144</v>
       </c>
       <c r="B394" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C394" s="0" t="s">
         <v>33</v>
@@ -15344,7 +15347,7 @@
         <v>144</v>
       </c>
       <c r="B395" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C395" s="0" t="s">
         <v>33</v>
@@ -15361,7 +15364,7 @@
         <v>144</v>
       </c>
       <c r="B396" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C396" s="0" t="s">
         <v>33</v>
@@ -15378,7 +15381,7 @@
         <v>144</v>
       </c>
       <c r="B397" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C397" s="0" t="s">
         <v>33</v>
@@ -15395,7 +15398,7 @@
         <v>144</v>
       </c>
       <c r="B398" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C398" s="0" t="s">
         <v>33</v>
@@ -15412,7 +15415,7 @@
         <v>144</v>
       </c>
       <c r="B399" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C399" s="0" t="s">
         <v>33</v>
@@ -15429,7 +15432,7 @@
         <v>144</v>
       </c>
       <c r="B400" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C400" s="0" t="s">
         <v>33</v>
@@ -15446,7 +15449,7 @@
         <v>144</v>
       </c>
       <c r="B401" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C401" s="0" t="s">
         <v>33</v>
@@ -15463,7 +15466,7 @@
         <v>144</v>
       </c>
       <c r="B402" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C402" s="0" t="s">
         <v>33</v>
@@ -15480,7 +15483,7 @@
         <v>144</v>
       </c>
       <c r="B403" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C403" s="0" t="s">
         <v>33</v>
@@ -15492,21 +15495,21 @@
         <v>131</v>
       </c>
     </row>
-    <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A404" s="0" t="s">
-        <v>144</v>
+    <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A404" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="B404" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="C404" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D404" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E404" s="0" t="s">
-        <v>131</v>
+        <v>51</v>
+      </c>
+      <c r="C404" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D404" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E404" s="16" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15514,7 +15517,7 @@
         <v>127</v>
       </c>
       <c r="B405" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C405" s="11" t="s">
         <v>21</v>
@@ -15528,13 +15531,13 @@
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="11" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B406" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C406" s="11" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D406" s="11" t="s">
         <v>128</v>
@@ -15548,7 +15551,7 @@
         <v>146</v>
       </c>
       <c r="B407" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C407" s="11" t="s">
         <v>29</v>
@@ -15561,17 +15564,17 @@
       </c>
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A408" s="11" t="s">
-        <v>146</v>
+      <c r="A408" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="B408" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C408" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D408" s="11" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="E408" s="16" t="s">
         <v>130</v>
@@ -15582,7 +15585,7 @@
         <v>139</v>
       </c>
       <c r="B409" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C409" s="11" t="s">
         <v>30</v>
@@ -15594,18 +15597,18 @@
         <v>130</v>
       </c>
     </row>
-    <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="410" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B410" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C410" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D410" s="11" t="s">
-        <v>141</v>
+        <v>31</v>
+      </c>
+      <c r="D410" s="15" t="s">
+        <v>145</v>
       </c>
       <c r="E410" s="16" t="s">
         <v>130</v>
@@ -15616,7 +15619,7 @@
         <v>144</v>
       </c>
       <c r="B411" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C411" s="11" t="s">
         <v>31</v>
@@ -15633,10 +15636,10 @@
         <v>144</v>
       </c>
       <c r="B412" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C412" s="11" t="s">
-        <v>31</v>
+        <v>51</v>
+      </c>
+      <c r="C412" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="D412" s="15" t="s">
         <v>145</v>
@@ -15650,7 +15653,7 @@
         <v>144</v>
       </c>
       <c r="B413" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C413" s="0" t="s">
         <v>32</v>
@@ -15667,10 +15670,10 @@
         <v>144</v>
       </c>
       <c r="B414" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C414" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D414" s="15" t="s">
         <v>145</v>
@@ -15684,7 +15687,7 @@
         <v>144</v>
       </c>
       <c r="B415" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C415" s="0" t="s">
         <v>33</v>
@@ -15696,21 +15699,21 @@
         <v>130</v>
       </c>
     </row>
-    <row r="416" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A416" s="0" t="s">
-        <v>144</v>
+    <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A416" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="B416" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C416" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D416" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E416" s="16" t="s">
-        <v>130</v>
+        <v>68</v>
+      </c>
+      <c r="C416" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D416" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E416" s="11" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15718,7 +15721,7 @@
         <v>127</v>
       </c>
       <c r="B417" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C417" s="11" t="s">
         <v>21</v>
@@ -15735,7 +15738,7 @@
         <v>127</v>
       </c>
       <c r="B418" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C418" s="11" t="s">
         <v>21</v>
@@ -15752,7 +15755,7 @@
         <v>127</v>
       </c>
       <c r="B419" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C419" s="11" t="s">
         <v>21</v>
@@ -15769,7 +15772,7 @@
         <v>127</v>
       </c>
       <c r="B420" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C420" s="11" t="s">
         <v>21</v>
@@ -15786,7 +15789,7 @@
         <v>127</v>
       </c>
       <c r="B421" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C421" s="11" t="s">
         <v>21</v>
@@ -15800,13 +15803,13 @@
     </row>
     <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="11" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B422" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C422" s="11" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D422" s="11" t="s">
         <v>128</v>
@@ -15820,7 +15823,7 @@
         <v>146</v>
       </c>
       <c r="B423" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C423" s="11" t="s">
         <v>29</v>
@@ -15837,7 +15840,7 @@
         <v>146</v>
       </c>
       <c r="B424" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C424" s="11" t="s">
         <v>29</v>
@@ -15854,7 +15857,7 @@
         <v>146</v>
       </c>
       <c r="B425" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C425" s="11" t="s">
         <v>29</v>
@@ -15871,7 +15874,7 @@
         <v>146</v>
       </c>
       <c r="B426" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C426" s="11" t="s">
         <v>29</v>
@@ -15888,7 +15891,7 @@
         <v>146</v>
       </c>
       <c r="B427" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C427" s="11" t="s">
         <v>29</v>
@@ -15901,17 +15904,17 @@
       </c>
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A428" s="11" t="s">
-        <v>146</v>
+      <c r="A428" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="B428" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C428" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D428" s="11" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="E428" s="11" t="s">
         <v>132</v>
@@ -15922,7 +15925,7 @@
         <v>139</v>
       </c>
       <c r="B429" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C429" s="11" t="s">
         <v>30</v>
@@ -15939,7 +15942,7 @@
         <v>139</v>
       </c>
       <c r="B430" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C430" s="11" t="s">
         <v>30</v>
@@ -15956,7 +15959,7 @@
         <v>139</v>
       </c>
       <c r="B431" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C431" s="11" t="s">
         <v>30</v>
@@ -15973,7 +15976,7 @@
         <v>139</v>
       </c>
       <c r="B432" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C432" s="11" t="s">
         <v>30</v>
@@ -15990,7 +15993,7 @@
         <v>139</v>
       </c>
       <c r="B433" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C433" s="11" t="s">
         <v>30</v>
@@ -16003,68 +16006,68 @@
       </c>
     </row>
     <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="0" t="s">
+      <c r="A434" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B434" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C434" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D434" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E434" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A435" s="0" t="s">
         <v>139</v>
-      </c>
-      <c r="B434" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C434" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D434" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="E434" s="11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="11" t="s">
-        <v>146</v>
       </c>
       <c r="B435" s="0" t="s">
         <v>34</v>
       </c>
       <c r="C435" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D435" s="11" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="E435" s="16" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A436" s="0" t="s">
-        <v>139</v>
+      <c r="A436" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="B436" s="0" t="s">
         <v>34</v>
       </c>
       <c r="C436" s="11" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D436" s="11" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="E436" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A437" s="11" t="s">
-        <v>127</v>
+    <row r="437" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A437" s="0" t="s">
+        <v>144</v>
       </c>
       <c r="B437" s="0" t="s">
         <v>34</v>
       </c>
       <c r="C437" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D437" s="11" t="s">
-        <v>128</v>
+        <v>31</v>
+      </c>
+      <c r="D437" s="15" t="s">
+        <v>145</v>
       </c>
       <c r="E437" s="16" t="s">
         <v>129</v>
@@ -16077,8 +16080,8 @@
       <c r="B438" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C438" s="11" t="s">
-        <v>31</v>
+      <c r="C438" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="D438" s="15" t="s">
         <v>145</v>
@@ -16095,7 +16098,7 @@
         <v>34</v>
       </c>
       <c r="C439" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D439" s="15" t="s">
         <v>145</v>
@@ -16104,76 +16107,76 @@
         <v>129</v>
       </c>
     </row>
-    <row r="440" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="0" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B440" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C440" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D440" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E440" s="16" t="s">
-        <v>129</v>
+        <v>159</v>
+      </c>
+      <c r="C440" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D440" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E440" s="0" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A441" s="0" t="s">
-        <v>139</v>
+      <c r="A441" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="B441" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C441" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D441" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E441" s="0" t="s">
         <v>160</v>
-      </c>
-      <c r="C441" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D441" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="E441" s="0" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="11" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B442" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="C442" s="11" t="s">
-        <v>21</v>
+        <v>159</v>
+      </c>
+      <c r="C442" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="D442" s="11" t="s">
         <v>128</v>
       </c>
       <c r="E442" s="0" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A443" s="11" t="s">
-        <v>146</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="443" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A443" s="0" t="s">
+        <v>144</v>
       </c>
       <c r="B443" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="C443" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D443" s="11" t="s">
-        <v>128</v>
+        <v>168</v>
+      </c>
+      <c r="C443" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D443" s="15" t="s">
+        <v>145</v>
       </c>
       <c r="E443" s="0" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F440"/>
+  <autoFilter ref="A1:F442"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>